<commit_message>
Part-1 Trainer's Classwork File
</commit_message>
<xml_diff>
--- a/Excel Part-1 (Trainer-157).xlsx
+++ b/Excel Part-1 (Trainer-157).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Business Analyst\USA BA 157\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AA28E8-4B7D-4854-AA13-BD197A57B5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA1B794-23EB-45C7-8D31-50F0C13B4573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,7 +521,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3593" uniqueCount="1374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3595" uniqueCount="1375">
   <si>
     <t>Text</t>
   </si>
@@ -4653,6 +4653,9 @@
   </si>
   <si>
     <t>Company DEFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -4947,7 +4950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5017,6 +5020,11 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5032,13 +5040,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6391,10 +6392,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="B3:H14"/>
+  <dimension ref="B3:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6404,103 +6405,88 @@
     <col min="5" max="5" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:9">
       <c r="B3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="48" t="s">
+    <row r="4" spans="2:9">
+      <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45" t="s">
+      <c r="E4" t="s">
         <v>1368</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="48" t="s">
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="48" t="s">
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="48" t="s">
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-    </row>
-    <row r="9" spans="2:8">
+    </row>
+    <row r="8" spans="2:9">
+      <c r="I8" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="2:8">
+      <c r="D9" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" s="14" t="s">
         <v>1369</v>
       </c>
-      <c r="C10" s="47" t="str">
+      <c r="C10" s="41" t="str">
         <f>TRIM(B10)</f>
         <v>Company ABC</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:9">
       <c r="B11" s="14" t="s">
         <v>1370</v>
       </c>
-      <c r="C11" s="47" t="str">
+      <c r="C11" s="41" t="str">
         <f t="shared" ref="C11:C14" si="0">TRIM(B11)</f>
         <v>Company XYZ</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:9">
       <c r="B12" s="14" t="s">
         <v>1371</v>
       </c>
-      <c r="C12" s="47" t="str">
+      <c r="C12" s="41" t="str">
         <f t="shared" si="0"/>
         <v>Company MNOP</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:9">
       <c r="B13" s="14" t="s">
         <v>1372</v>
       </c>
-      <c r="C13" s="47" t="str">
+      <c r="C13" s="41" t="str">
         <f t="shared" si="0"/>
         <v>Company PQRS</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:9">
       <c r="B14" s="14" t="s">
         <v>1373</v>
       </c>
-      <c r="C14" s="47" t="str">
+      <c r="C14" s="41" t="str">
         <f t="shared" si="0"/>
         <v>Company DEFG</v>
       </c>
@@ -41243,7 +41229,7 @@
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="39">
         <f>AVERAGE(E4:G13)</f>
         <v>63.44</v>
       </c>
@@ -41449,26 +41435,26 @@
       </c>
     </row>
     <row r="16" spans="2:19" ht="15.5">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="42" t="s">
         <v>1331</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="34" t="s">
@@ -42471,7 +42457,7 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="L2" s="45">
+      <c r="L2">
         <v>500</v>
       </c>
     </row>
@@ -42479,7 +42465,7 @@
       <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="L3" t="s">
         <v>1343</v>
       </c>
     </row>
@@ -42494,7 +42480,7 @@
       <c r="F4">
         <v>200</v>
       </c>
-      <c r="L4" s="45" t="b">
+      <c r="L4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -42506,7 +42492,7 @@
         <f t="shared" ref="D5:D6" si="0">$F$4&gt;C5</f>
         <v>1</v>
       </c>
-      <c r="L5" s="45" t="b">
+      <c r="L5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -42520,21 +42506,21 @@
       </c>
     </row>
     <row r="10" spans="3:18" ht="15.5">
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="43" t="s">
         <v>1304</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
     </row>
     <row r="11" spans="3:18">
       <c r="C11" s="30" t="s">
@@ -42587,40 +42573,40 @@
       <c r="C12" s="33" t="s">
         <v>1318</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="40">
         <v>6250</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="40">
         <v>3710</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="40">
         <v>5478.75</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="40">
         <v>4897.5</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="40">
         <v>3265</v>
       </c>
-      <c r="I12" s="46">
+      <c r="I12" s="40">
         <v>3681.25</v>
       </c>
-      <c r="J12" s="46">
+      <c r="J12" s="40">
         <v>5382.5</v>
       </c>
-      <c r="K12" s="46">
+      <c r="K12" s="40">
         <v>2906.25</v>
       </c>
-      <c r="L12" s="46">
+      <c r="L12" s="40">
         <v>6152.5</v>
       </c>
-      <c r="M12" s="46">
+      <c r="M12" s="40">
         <v>2895</v>
       </c>
-      <c r="N12" s="46">
+      <c r="N12" s="40">
         <v>4283.75</v>
       </c>
-      <c r="O12" s="46">
+      <c r="O12" s="40">
         <v>1900</v>
       </c>
     </row>
@@ -42628,43 +42614,43 @@
       <c r="C13" s="33" t="s">
         <v>1319</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="40">
         <v>4241.25</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="40">
         <v>3790</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="40">
         <v>4152.5</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="40">
         <v>5383.75</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="40">
         <v>4817.5</v>
       </c>
-      <c r="I13" s="46">
+      <c r="I13" s="40">
         <v>5808.75</v>
       </c>
-      <c r="J13" s="46">
+      <c r="J13" s="40">
         <v>6233.75</v>
       </c>
-      <c r="K13" s="46">
+      <c r="K13" s="40">
         <v>3087.5</v>
       </c>
-      <c r="L13" s="46">
+      <c r="L13" s="40">
         <v>2535</v>
       </c>
-      <c r="M13" s="46">
+      <c r="M13" s="40">
         <v>4508.75</v>
       </c>
-      <c r="N13" s="46">
+      <c r="N13" s="40">
         <v>2146.25</v>
       </c>
-      <c r="O13" s="46">
+      <c r="O13" s="40">
         <v>6188.75</v>
       </c>
-      <c r="R13" s="46">
+      <c r="R13" s="40">
         <v>1.25</v>
       </c>
     </row>
@@ -42672,40 +42658,40 @@
       <c r="C14" s="33" t="s">
         <v>1320</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="40">
         <v>5175</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="40">
         <v>2550</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="40">
         <v>6223.75</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="40">
         <v>5228.75</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="40">
         <v>4225</v>
       </c>
-      <c r="I14" s="46">
+      <c r="I14" s="40">
         <v>6053.75</v>
       </c>
-      <c r="J14" s="46">
+      <c r="J14" s="40">
         <v>6162.5</v>
       </c>
-      <c r="K14" s="46">
+      <c r="K14" s="40">
         <v>1892.5</v>
       </c>
-      <c r="L14" s="46">
+      <c r="L14" s="40">
         <v>2180</v>
       </c>
-      <c r="M14" s="46">
+      <c r="M14" s="40">
         <v>2751.25</v>
       </c>
-      <c r="N14" s="46">
+      <c r="N14" s="40">
         <v>2518.75</v>
       </c>
-      <c r="O14" s="46">
+      <c r="O14" s="40">
         <v>2871.25</v>
       </c>
     </row>
@@ -42713,40 +42699,40 @@
       <c r="C15" s="33" t="s">
         <v>1321</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="40">
         <v>4687.5</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="40">
         <v>4826.25</v>
       </c>
-      <c r="F15" s="46">
+      <c r="F15" s="40">
         <v>4885</v>
       </c>
-      <c r="G15" s="46">
+      <c r="G15" s="40">
         <v>6238.75</v>
       </c>
-      <c r="H15" s="46">
+      <c r="H15" s="40">
         <v>3153.75</v>
       </c>
-      <c r="I15" s="46">
+      <c r="I15" s="40">
         <v>4881.25</v>
       </c>
-      <c r="J15" s="46">
+      <c r="J15" s="40">
         <v>3723.75</v>
       </c>
-      <c r="K15" s="46">
+      <c r="K15" s="40">
         <v>3056.25</v>
       </c>
-      <c r="L15" s="46">
+      <c r="L15" s="40">
         <v>4832.5</v>
       </c>
-      <c r="M15" s="46">
+      <c r="M15" s="40">
         <v>2393.75</v>
       </c>
-      <c r="N15" s="46">
+      <c r="N15" s="40">
         <v>2326.25</v>
       </c>
-      <c r="O15" s="46">
+      <c r="O15" s="40">
         <v>6161.25</v>
       </c>
     </row>
@@ -42754,40 +42740,40 @@
       <c r="C16" s="33" t="s">
         <v>1322</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="40">
         <v>3830</v>
       </c>
-      <c r="E16" s="46">
+      <c r="E16" s="40">
         <v>5942.5</v>
       </c>
-      <c r="F16" s="46">
+      <c r="F16" s="40">
         <v>4337.5</v>
       </c>
-      <c r="G16" s="46">
+      <c r="G16" s="40">
         <v>5937.5</v>
       </c>
-      <c r="H16" s="46">
+      <c r="H16" s="40">
         <v>3366.25</v>
       </c>
-      <c r="I16" s="46">
+      <c r="I16" s="40">
         <v>2160</v>
       </c>
-      <c r="J16" s="46">
+      <c r="J16" s="40">
         <v>4225</v>
       </c>
-      <c r="K16" s="46">
+      <c r="K16" s="40">
         <v>2200</v>
       </c>
-      <c r="L16" s="46">
+      <c r="L16" s="40">
         <v>4125</v>
       </c>
-      <c r="M16" s="46">
+      <c r="M16" s="40">
         <v>4168.75</v>
       </c>
-      <c r="N16" s="46">
+      <c r="N16" s="40">
         <v>5877.5</v>
       </c>
-      <c r="O16" s="46">
+      <c r="O16" s="40">
         <v>2770</v>
       </c>
     </row>
@@ -42795,40 +42781,40 @@
       <c r="C17" s="33" t="s">
         <v>1323</v>
       </c>
-      <c r="D17" s="46">
+      <c r="D17" s="40">
         <v>5726.25</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E17" s="40">
         <v>4693.75</v>
       </c>
-      <c r="F17" s="46">
+      <c r="F17" s="40">
         <v>3276.25</v>
       </c>
-      <c r="G17" s="46">
+      <c r="G17" s="40">
         <v>4571.25</v>
       </c>
-      <c r="H17" s="46">
+      <c r="H17" s="40">
         <v>5231.25</v>
       </c>
-      <c r="I17" s="46">
+      <c r="I17" s="40">
         <v>3290</v>
       </c>
-      <c r="J17" s="46">
+      <c r="J17" s="40">
         <v>4895</v>
       </c>
-      <c r="K17" s="46">
+      <c r="K17" s="40">
         <v>2817.5</v>
       </c>
-      <c r="L17" s="46">
+      <c r="L17" s="40">
         <v>5941.25</v>
       </c>
-      <c r="M17" s="46">
+      <c r="M17" s="40">
         <v>5957.5</v>
       </c>
-      <c r="N17" s="46">
+      <c r="N17" s="40">
         <v>3347.5</v>
       </c>
-      <c r="O17" s="46">
+      <c r="O17" s="40">
         <v>4991.25</v>
       </c>
     </row>
@@ -42836,40 +42822,40 @@
       <c r="C18" s="33" t="s">
         <v>1324</v>
       </c>
-      <c r="D18" s="46">
+      <c r="D18" s="40">
         <v>2726.25</v>
       </c>
-      <c r="E18" s="46">
+      <c r="E18" s="40">
         <v>5265</v>
       </c>
-      <c r="F18" s="46">
+      <c r="F18" s="40">
         <v>6001.25</v>
       </c>
-      <c r="G18" s="46">
+      <c r="G18" s="40">
         <v>4556.25</v>
       </c>
-      <c r="H18" s="46">
+      <c r="H18" s="40">
         <v>2636.25</v>
       </c>
-      <c r="I18" s="46">
+      <c r="I18" s="40">
         <v>3305</v>
       </c>
-      <c r="J18" s="46">
+      <c r="J18" s="40">
         <v>4070</v>
       </c>
-      <c r="K18" s="46">
+      <c r="K18" s="40">
         <v>4731.25</v>
       </c>
-      <c r="L18" s="46">
+      <c r="L18" s="40">
         <v>3405</v>
       </c>
-      <c r="M18" s="46">
+      <c r="M18" s="40">
         <v>3958.75</v>
       </c>
-      <c r="N18" s="46">
+      <c r="N18" s="40">
         <v>4888.75</v>
       </c>
-      <c r="O18" s="46">
+      <c r="O18" s="40">
         <v>5922.5</v>
       </c>
     </row>
@@ -42877,40 +42863,40 @@
       <c r="C19" s="33" t="s">
         <v>1325</v>
       </c>
-      <c r="D19" s="46">
+      <c r="D19" s="40">
         <v>4263.75</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="40">
         <v>1926.25</v>
       </c>
-      <c r="F19" s="46">
+      <c r="F19" s="40">
         <v>3118.75</v>
       </c>
-      <c r="G19" s="46">
+      <c r="G19" s="40">
         <v>2705</v>
       </c>
-      <c r="H19" s="46">
+      <c r="H19" s="40">
         <v>5851.25</v>
       </c>
-      <c r="I19" s="46">
+      <c r="I19" s="40">
         <v>3112.5</v>
       </c>
-      <c r="J19" s="46">
+      <c r="J19" s="40">
         <v>2068.75</v>
       </c>
-      <c r="K19" s="46">
+      <c r="K19" s="40">
         <v>5565</v>
       </c>
-      <c r="L19" s="46">
+      <c r="L19" s="40">
         <v>5341.25</v>
       </c>
-      <c r="M19" s="46">
+      <c r="M19" s="40">
         <v>2907.5</v>
       </c>
-      <c r="N19" s="46">
+      <c r="N19" s="40">
         <v>6007.5</v>
       </c>
-      <c r="O19" s="46">
+      <c r="O19" s="40">
         <v>3840</v>
       </c>
     </row>
@@ -42918,40 +42904,40 @@
       <c r="C20" s="33" t="s">
         <v>1326</v>
       </c>
-      <c r="D20" s="46">
+      <c r="D20" s="40">
         <v>5281.25</v>
       </c>
-      <c r="E20" s="46">
+      <c r="E20" s="40">
         <v>2423.75</v>
       </c>
-      <c r="F20" s="46">
+      <c r="F20" s="40">
         <v>4530</v>
       </c>
-      <c r="G20" s="46">
+      <c r="G20" s="40">
         <v>3162.5</v>
       </c>
-      <c r="H20" s="46">
+      <c r="H20" s="40">
         <v>5010</v>
       </c>
-      <c r="I20" s="46">
+      <c r="I20" s="40">
         <v>3020</v>
       </c>
-      <c r="J20" s="46">
+      <c r="J20" s="40">
         <v>2778.75</v>
       </c>
-      <c r="K20" s="46">
+      <c r="K20" s="40">
         <v>2780</v>
       </c>
-      <c r="L20" s="46">
+      <c r="L20" s="40">
         <v>3555</v>
       </c>
-      <c r="M20" s="46">
+      <c r="M20" s="40">
         <v>5300</v>
       </c>
-      <c r="N20" s="46">
+      <c r="N20" s="40">
         <v>3970</v>
       </c>
-      <c r="O20" s="46">
+      <c r="O20" s="40">
         <v>3242.5</v>
       </c>
     </row>
@@ -42959,40 +42945,40 @@
       <c r="C21" s="33" t="s">
         <v>1327</v>
       </c>
-      <c r="D21" s="46">
+      <c r="D21" s="40">
         <v>5172.5</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="40">
         <v>1966.25</v>
       </c>
-      <c r="F21" s="46">
+      <c r="F21" s="40">
         <v>4971.25</v>
       </c>
-      <c r="G21" s="46">
+      <c r="G21" s="40">
         <v>2473.75</v>
       </c>
-      <c r="H21" s="46">
+      <c r="H21" s="40">
         <v>2135</v>
       </c>
-      <c r="I21" s="46">
+      <c r="I21" s="40">
         <v>5381.25</v>
       </c>
-      <c r="J21" s="46">
+      <c r="J21" s="40">
         <v>2482.5</v>
       </c>
-      <c r="K21" s="46">
+      <c r="K21" s="40">
         <v>3648.75</v>
       </c>
-      <c r="L21" s="46">
+      <c r="L21" s="40">
         <v>4286.25</v>
       </c>
-      <c r="M21" s="46">
+      <c r="M21" s="40">
         <v>3208.75</v>
       </c>
-      <c r="N21" s="46">
+      <c r="N21" s="40">
         <v>1975</v>
       </c>
-      <c r="O21" s="46">
+      <c r="O21" s="40">
         <v>2918.75</v>
       </c>
     </row>
@@ -43000,40 +42986,40 @@
       <c r="C22" s="33" t="s">
         <v>1328</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D22" s="40">
         <v>4361.25</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="40">
         <v>5561.25</v>
       </c>
-      <c r="F22" s="46">
+      <c r="F22" s="40">
         <v>5771.25</v>
       </c>
-      <c r="G22" s="46">
+      <c r="G22" s="40">
         <v>5551.25</v>
       </c>
-      <c r="H22" s="46">
+      <c r="H22" s="40">
         <v>5870</v>
       </c>
-      <c r="I22" s="46">
+      <c r="I22" s="40">
         <v>4106.25</v>
       </c>
-      <c r="J22" s="46">
+      <c r="J22" s="40">
         <v>3697.5</v>
       </c>
-      <c r="K22" s="46">
+      <c r="K22" s="40">
         <v>3721.25</v>
       </c>
-      <c r="L22" s="46">
+      <c r="L22" s="40">
         <v>2228.75</v>
       </c>
-      <c r="M22" s="46">
+      <c r="M22" s="40">
         <v>2141.25</v>
       </c>
-      <c r="N22" s="46">
+      <c r="N22" s="40">
         <v>3233.75</v>
       </c>
-      <c r="O22" s="46">
+      <c r="O22" s="40">
         <v>3960</v>
       </c>
     </row>
@@ -43041,40 +43027,40 @@
       <c r="C23" s="33" t="s">
         <v>1329</v>
       </c>
-      <c r="D23" s="46">
+      <c r="D23" s="40">
         <v>2628.75</v>
       </c>
-      <c r="E23" s="46">
+      <c r="E23" s="40">
         <v>5852.5</v>
       </c>
-      <c r="F23" s="46">
+      <c r="F23" s="40">
         <v>4867.5</v>
       </c>
-      <c r="G23" s="46">
+      <c r="G23" s="40">
         <v>3961.25</v>
       </c>
-      <c r="H23" s="46">
+      <c r="H23" s="40">
         <v>3475</v>
       </c>
-      <c r="I23" s="46">
+      <c r="I23" s="40">
         <v>5575</v>
       </c>
-      <c r="J23" s="46">
+      <c r="J23" s="40">
         <v>3307.5</v>
       </c>
-      <c r="K23" s="46">
+      <c r="K23" s="40">
         <v>5632.5</v>
       </c>
-      <c r="L23" s="46">
+      <c r="L23" s="40">
         <v>2350</v>
       </c>
-      <c r="M23" s="46">
+      <c r="M23" s="40">
         <v>5198.75</v>
       </c>
-      <c r="N23" s="46">
+      <c r="N23" s="40">
         <v>2553.75</v>
       </c>
-      <c r="O23" s="46">
+      <c r="O23" s="40">
         <v>3678.75</v>
       </c>
     </row>
@@ -43082,40 +43068,40 @@
       <c r="C24" s="33" t="s">
         <v>1330</v>
       </c>
-      <c r="D24" s="46">
+      <c r="D24" s="40">
         <v>3183.75</v>
       </c>
-      <c r="E24" s="46">
+      <c r="E24" s="40">
         <v>5645</v>
       </c>
-      <c r="F24" s="46">
+      <c r="F24" s="40">
         <v>4722.5</v>
       </c>
-      <c r="G24" s="46">
+      <c r="G24" s="40">
         <v>4643.75</v>
       </c>
-      <c r="H24" s="46">
+      <c r="H24" s="40">
         <v>4885</v>
       </c>
-      <c r="I24" s="46">
+      <c r="I24" s="40">
         <v>5658.75</v>
       </c>
-      <c r="J24" s="46">
+      <c r="J24" s="40">
         <v>4631.25</v>
       </c>
-      <c r="K24" s="46">
+      <c r="K24" s="40">
         <v>5443.75</v>
       </c>
-      <c r="L24" s="46">
+      <c r="L24" s="40">
         <v>5948.75</v>
       </c>
-      <c r="M24" s="46">
+      <c r="M24" s="40">
         <v>2497.5</v>
       </c>
-      <c r="N24" s="46">
+      <c r="N24" s="40">
         <v>2301.25</v>
       </c>
-      <c r="O24" s="46">
+      <c r="O24" s="40">
         <v>2180</v>
       </c>
     </row>
@@ -43381,21 +43367,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11">
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41" t="s">
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="43" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="46" t="s">
         <v>1339</v>
       </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" s="19" t="s">

</xml_diff>